<commit_message>
Data collection for 2018. Split data into testing and training.
70 percent of 2018 data and 70 percent of 2017 data make up all training data
30 percent of 2018 and 30 percent of 2017 make up all testing data
data is split by position, X, Y, training, testing (phew)
</commit_message>
<xml_diff>
--- a/2018_data/Adam_Shaheen_TE_2018.xlsx
+++ b/2018_data/Adam_Shaheen_TE_2018.xlsx
@@ -1,57 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>rec_yds</t>
-  </si>
-  <si>
-    <t>rec_td</t>
-  </si>
-  <si>
-    <t>fumbles</t>
-  </si>
-  <si>
-    <t>fantasy points</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -66,35 +46,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -382,130 +353,144 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>rec_yds</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>rec_td</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>fumbles</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>fantasy points</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>6.5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="1">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3">
+      <c r="B5" t="n">
+        <v>39</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>3.9</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="n">
+        <v>4</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>6.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="1">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>39</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>3.9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
+      <c r="B7" t="n">
+        <v>0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" t="n">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>